<commit_message>
bảng phân công nhiệm vụ
</commit_message>
<xml_diff>
--- a/baitap_project_ST6.xlsx
+++ b/baitap_project_ST6.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t xml:space="preserve">Yêu cầu: Nhóm tối thiểu 5 và tối đa 10 thanh viên tự chọn, Phân công nhiệm vụ mỗi thành viên vào sheet "Bang_Phan_Cong_Nhiem_Vu" và phối hợp hoàn thành thử thách bên dưới. Nhóm trưởng tạo 01 Repository trên github để chứa project (API &amp; APP) và add các thành viên nhóm vào, mỗi thành viên phải comment code của mình và commit lên nhánh của mình trong project. Trưởng nhóm sẽ merge lại trên nhóm chính. Giao diện bài tập chỉ là mẫu, các nhóm chọn dữ liệu riêng của mỗi nhóm. Chụp giao diện của nhóm bỏ vào Readme trên github. </t>
   </si>
@@ -93,7 +93,7 @@
     <t>Nguyễn Hoàng Anh Khoa</t>
   </si>
   <si>
-    <t>Thiết kế giao diện Intro, giao diện bottomAppBarr, logic nút bắt đầu, login activity, merge code, tạo repo</t>
+    <t>Thiết kế giao diện Intro, giao diện bottomAppBar, logic nút bắt đầu, login activity, merge code, tạo repo</t>
   </si>
   <si>
     <t>Châu Văn Thân</t>
@@ -106,6 +106,36 @@
   </si>
   <si>
     <t>Thiết api, code activity cho giao diện cho đăng ký và otp</t>
+  </si>
+  <si>
+    <t>Nguyễn Lý Hùng</t>
+  </si>
+  <si>
+    <t>Viết API lấy các category theo chiều ngang , viết logic gọi api hiển thị thông tin category lên màn hình, merge code</t>
+  </si>
+  <si>
+    <t>Lê Đình Lộc</t>
+  </si>
+  <si>
+    <t>Viết API lấy thông tin user , gọi api hiển thị thông tin user lên màn hình</t>
+  </si>
+  <si>
+    <t>Võ Văn Nam</t>
+  </si>
+  <si>
+    <t>Thiết kế giao diện  màn hình chính, tinh chỉnh bottomAppBar</t>
+  </si>
+  <si>
+    <t>Nguyễn Tuấn Thành</t>
+  </si>
+  <si>
+    <t>Xây dựng chức năng lấy tất cả sản phẩm theo từng category được sắp xếp tăng dần theo giá bán hiển thị dạng lưới</t>
+  </si>
+  <si>
+    <t>Huỳnh Thái Toàn</t>
+  </si>
+  <si>
+    <t>Thiết kế giao diện đăng nhập và viết API đăng nhập</t>
   </si>
 </sst>
 </file>
@@ -118,7 +148,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -133,6 +163,12 @@
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.25"/>
+      <color rgb="FF081B3A"/>
+      <name val="Segoe UI"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -581,152 +617,153 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1146,88 +1183,88 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
   <sheetData>
     <row r="3" ht="59.4" customHeight="1" spans="14:21">
-      <c r="N3" s="2" t="s">
+      <c r="N3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
     </row>
     <row r="4" ht="46.2" customHeight="1" spans="14:21">
-      <c r="N4" s="3" t="s">
+      <c r="N4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
     </row>
     <row r="5" ht="17.4" customHeight="1" spans="14:21">
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
     </row>
     <row r="6" spans="14:21">
-      <c r="N6" s="4" t="s">
+      <c r="N6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
     </row>
     <row r="7" spans="14:21">
-      <c r="N7" s="4" t="s">
+      <c r="N7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
     </row>
     <row r="8" spans="14:21">
-      <c r="N8" s="4" t="s">
+      <c r="N8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
-      <c r="U8" s="4"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
     </row>
     <row r="9" spans="14:21">
-      <c r="N9" s="4" t="s">
+      <c r="N9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="4"/>
-      <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="4"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
     </row>
     <row r="10" spans="14:14">
       <c r="N10" t="s">
@@ -1277,14 +1314,14 @@
   <dimension ref="A2:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" outlineLevelCol="4"/>
   <cols>
     <col min="2" max="2" width="12.4" customWidth="1"/>
     <col min="3" max="3" width="21.9" customWidth="1"/>
-    <col min="4" max="4" width="90.4" customWidth="1"/>
+    <col min="4" max="4" width="108" customWidth="1"/>
     <col min="5" max="5" width="26.3" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1360,29 +1397,74 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
+      <c r="B8">
+        <v>22110337</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="B9">
+        <v>22110369</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
+      <c r="B10">
+        <v>22110379</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" ht="16.2" spans="1:4">
       <c r="A11">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
+      <c r="B11">
+        <v>22110418</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>8</v>
+      </c>
+      <c r="B12">
+        <v>22110436</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>